<commit_message>
Inscrição usando CPF e ID
</commit_message>
<xml_diff>
--- a/docs/projeto.xlsx
+++ b/docs/projeto.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="106">
   <si>
     <t>Controller</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Users</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>Formulário de cadastro de novo usuário.</t>
   </si>
   <si>
-    <t>key</t>
-  </si>
-  <si>
     <t>Ativação de um usuário cadastrado.</t>
   </si>
   <si>
@@ -343,6 +337,9 @@
   </si>
   <si>
     <t>Página de inscrição do evento</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -444,10 +441,10 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G32" totalsRowShown="0">
   <autoFilter ref="A1:G32"/>
-  <sortState ref="A2:H24">
-    <sortCondition ref="A2:A24"/>
-    <sortCondition ref="B2:B24"/>
-    <sortCondition ref="C2:C24"/>
+  <sortState ref="A2:G32">
+    <sortCondition ref="A2:A32"/>
+    <sortCondition ref="B2:B32"/>
+    <sortCondition ref="C2:C32"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Module"/>
@@ -814,144 +811,144 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -979,134 +976,134 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
         <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
         <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
         <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
         <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1126,9 +1123,7 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1143,42 +1138,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G2" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1187,19 +1182,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1208,22 +1203,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1232,22 +1227,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1256,19 +1251,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
         <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
       </c>
       <c r="G6" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1277,19 +1272,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1298,22 +1293,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1322,22 +1317,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1346,19 +1341,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
         <v>48</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
       </c>
       <c r="G10" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1367,19 +1362,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1388,22 +1383,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1412,22 +1407,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1436,19 +1431,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
         <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>49</v>
       </c>
       <c r="G14" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1457,19 +1452,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
       </c>
       <c r="G15" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1478,386 +1473,386 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Auth.login</v>
+        <v>99</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.boleto</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Auth.logout</v>
+        <v>100</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.detail</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Index.activate</v>
+        <v>102</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.inscricao</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Index.forgot</v>
+        <v>104</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.signup</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G20" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Index.index</v>
+        <v>TenilUser\Controller\Auth.login</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G21" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Index.register</v>
+        <v>TenilUser\Controller\Auth.logout</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G22" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Index.reset</v>
+        <v>TenilUser\Controller\Profile.edit</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G23" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Profile.edit</v>
+        <v>TenilUser\Controller\Profile.index</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G24" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Profile.index</v>
+        <v>TenilUser\Controller\User.activate</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Users.add</v>
+        <v>TenilUser\Controller\User.add</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G26" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Users.delete</v>
+        <v>TenilUser\Controller\User.delete</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Users.edit</v>
+        <v>TenilUser\Controller\User.edit</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="1" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilUser\Controller\Users.index</v>
+        <v>60</v>
+      </c>
+      <c r="G28" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\User.forgot</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="1" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilEvento\Controller\Eventos.boleto</v>
+        <v>56</v>
+      </c>
+      <c r="G29" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
         <v>48</v>
       </c>
-      <c r="E30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" t="s">
-        <v>102</v>
-      </c>
       <c r="G30" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilEvento\Controller\Eventos.detail</v>
+        <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>104</v>
-      </c>
-      <c r="G31" s="1" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilEvento\Controller\Eventos.inscricao</v>
+        <v>57</v>
+      </c>
+      <c r="G31" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\User.register</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="1" t="str">
-        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
-        <v>TenilEvento\Controller\Eventos.signup</v>
+        <v>60</v>
+      </c>
+      <c r="G32" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilUser\Controller\User.reset</v>
       </c>
     </row>
   </sheetData>
@@ -1884,18 +1879,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Envio de e-mail BCC 2. Lista de inscrições 3. Criação de partials
</commit_message>
<xml_diff>
--- a/docs/projeto.xlsx
+++ b/docs/projeto.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="117">
   <si>
     <t>Controller</t>
   </si>
@@ -111,9 +111,6 @@
     <t>tenil-acl-admin</t>
   </si>
   <si>
-    <t>/admin/acl</t>
-  </si>
-  <si>
     <t>/[:controller[/:action[/:id]]]</t>
   </si>
   <si>
@@ -340,6 +337,42 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>/acl</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>Criação de um novo evento</t>
+  </si>
+  <si>
+    <t>Lista todos itens cadastrados</t>
+  </si>
+  <si>
+    <t>id, cpf</t>
+  </si>
+  <si>
+    <t>retorno</t>
+  </si>
+  <si>
+    <t>Faz upload do arquivo de retorno</t>
+  </si>
+  <si>
+    <t>inscricoes</t>
+  </si>
+  <si>
+    <t>Lista as inscrições em um evento</t>
+  </si>
+  <si>
+    <t>Editar um Evento</t>
+  </si>
+  <si>
+    <t>Detralha um Evento</t>
+  </si>
+  <si>
+    <t>Exclui um Evento</t>
   </si>
 </sst>
 </file>
@@ -439,8 +472,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G32" totalsRowShown="0">
-  <autoFilter ref="A1:G32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G39" totalsRowShown="0">
+  <autoFilter ref="A1:G39">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Eventos"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:G32">
     <sortCondition ref="A2:A32"/>
     <sortCondition ref="B2:B32"/>
@@ -796,7 +835,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -874,16 +913,16 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -891,30 +930,30 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -922,33 +961,33 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>69</v>
-      </c>
-      <c r="E8" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -976,10 +1015,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -987,32 +1026,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1020,10 +1059,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1031,21 +1070,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -1053,57 +1092,57 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
         <v>89</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>93</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
         <v>95</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>96</v>
-      </c>
-      <c r="C13" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1121,9 +1160,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1147,19 +1188,19 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1170,301 +1211,301 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>Application\Controller\Index.index</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Privileges.add</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Privileges.delete</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Privileges.edit</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Privileges.index</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Resouces.add</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Resouces.delete</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Resouces.edit</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
       <c r="G10" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Resouces.index</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Roles.add</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Roles.delete</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Roles.edit</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
         <v>47</v>
       </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
       <c r="G14" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilAcl\Controller\Roles.index</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" t="s">
-        <v>44</v>
       </c>
       <c r="G15" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1473,22 +1514,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
         <v>98</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>99</v>
       </c>
       <c r="G16" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1497,22 +1538,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1521,22 +1562,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
         <v>101</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" t="s">
-        <v>102</v>
       </c>
       <c r="G18" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
@@ -1545,52 +1586,52 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
         <v>103</v>
       </c>
-      <c r="D19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" t="s">
-        <v>104</v>
-      </c>
       <c r="G19" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilEvento\Controller\Eventos.signup</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\Auth.login</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -1599,260 +1640,419 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\Auth.logout</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\Profile.edit</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\Profile.index</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.activate</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G25" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.add</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.delete</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G27" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.edit</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G28" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.forgot</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="F30" t="s">
-        <v>48</v>
-      </c>
       <c r="G30" s="1" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.register</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
         <v>59</v>
       </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" t="s">
-        <v>60</v>
-      </c>
       <c r="G32" t="str">
         <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
         <v>TenilUser\Controller\User.reset</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.create</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.list</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.edit</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.detail</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.delete</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.retorno</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f xml:space="preserve"> CONCATENATE(Tabela4[[#This Row],[Module]],"\Controller\",Tabela4[[#This Row],[Controller]],".",Tabela4[[#This Row],[Action]])</f>
+        <v>TenilEvento\Controller\Eventos.inscricoes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação de estrutura de menu usando zend\navigation
</commit_message>
<xml_diff>
--- a/docs/projeto.xlsx
+++ b/docs/projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -835,7 +835,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G16" sqref="G16:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organização de arquivos das pastas.
</commit_message>
<xml_diff>
--- a/docs/projeto.xlsx
+++ b/docs/projeto.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\rede.cb.org.br\www\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\cloud.tenil.com.br\www\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -473,13 +473,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:G39" totalsRowShown="0">
-  <autoFilter ref="A1:G39">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Eventos"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G39"/>
   <sortState ref="A2:G32">
     <sortCondition ref="A2:A32"/>
     <sortCondition ref="B2:B32"/>
@@ -1163,7 +1157,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G39"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1221,7 +1215,7 @@
         <v>Application\Controller\Index.index</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1242,7 +1236,7 @@
         <v>TenilAcl\Controller\Privileges.add</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1266,7 +1260,7 @@
         <v>TenilAcl\Controller\Privileges.delete</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1290,7 +1284,7 @@
         <v>TenilAcl\Controller\Privileges.edit</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1311,7 +1305,7 @@
         <v>TenilAcl\Controller\Privileges.index</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1332,7 +1326,7 @@
         <v>TenilAcl\Controller\Resouces.add</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1356,7 +1350,7 @@
         <v>TenilAcl\Controller\Resouces.delete</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1380,7 +1374,7 @@
         <v>TenilAcl\Controller\Resouces.edit</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1401,7 +1395,7 @@
         <v>TenilAcl\Controller\Resouces.index</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1422,7 +1416,7 @@
         <v>TenilAcl\Controller\Roles.add</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1446,7 +1440,7 @@
         <v>TenilAcl\Controller\Roles.delete</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1470,7 +1464,7 @@
         <v>TenilAcl\Controller\Roles.edit</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1491,7 +1485,7 @@
         <v>TenilAcl\Controller\Roles.index</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1608,7 +1602,7 @@
         <v>TenilEvento\Controller\Eventos.signup</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1623,7 @@
         <v>TenilUser\Controller\Auth.login</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1650,7 +1644,7 @@
         <v>TenilUser\Controller\Auth.logout</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1674,7 +1668,7 @@
         <v>TenilUser\Controller\Profile.edit</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1695,7 +1689,7 @@
         <v>TenilUser\Controller\Profile.index</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1719,7 +1713,7 @@
         <v>TenilUser\Controller\User.activate</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1740,7 +1734,7 @@
         <v>TenilUser\Controller\User.add</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1764,7 +1758,7 @@
         <v>TenilUser\Controller\User.delete</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1788,7 +1782,7 @@
         <v>TenilUser\Controller\User.edit</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>TenilUser\Controller\User.forgot</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1830,7 +1824,7 @@
         <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1851,7 +1845,7 @@
         <v>TenilUser\Controller\User.index</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1872,7 +1866,7 @@
         <v>TenilUser\Controller\User.register</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>

</xml_diff>